<commit_message>
add xlsx for ini file
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/EffectData.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/EffectData.xlsx
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add configure for function state
Former-commit-id: e4f492e6498b7c8b025a5905a71088847050dce0 [formerly dcff9b1f5208c3be0b8c3ae96ac27b73f1812635]
Former-commit-id: dc289dc7f9de93503ab3930e4cac0c244250ad9f
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/EffectData.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/EffectData.xlsx
@@ -1,144 +1,104 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="7905"/>
+    <workbookView windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
+  <extLst/>
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="EffectData" type="4" refreshedVersion="0" background="1">
-    <webPr xml="1" sourceData="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\EffectData.xml" htmlTables="1" htmlFormat="all"/>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31">
   <si>
     <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MAXHP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MAXSP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SpRegenTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ATK_VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DEF_VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DODGE_VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CRITICAL_VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>HPREGEN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CRITICAL_RATIO_VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>RESIST_VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DEF_CRITICAL_RATIO_VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DEF_HALT_VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DEF_SLOW_VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DEF_SILENCE_VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DEF_DIZZY_VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DEF_FREZE_VALUE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MOVE_SPEED</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ATK_SPEED</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>EQUIP_SCALE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ESSENCE_SCALE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>GOLD_SCALE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PHYSICAL_BREAK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>VPREGEN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MAXHP_ADD_RATE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ATK_ADD_RATE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DEF_ADD_RATE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CRITICAL_ADD_RATE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PlayerAtt1</t>
@@ -153,22 +113,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,8 +151,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -201,167 +179,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
+    <cellStyle name="百分比" xfId="4" builtinId="5"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
-<MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema1">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="XML">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Object" form="unqualified">
-              <xsd:complexType>
-                <xsd:attribute name="ID" form="unqualified" type="xsd:string"/>
-                <xsd:attribute name="MAXHP" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="MAXSP" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="SpRegenTime" form="unqualified" type="xsd:string"/>
-                <xsd:attribute name="ATK_VALUE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="DEF_VALUE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="DODGE_VALUE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="CRITICAL_VALUE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="HPREGEN" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="CRITICAL_RATIO_VALUE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="RESIST_VALUE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="DEF_CRITICAL_RATIO_VALUE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="DEF_HALT_VALUE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="DEF_SLOW_VALUE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="DEF_SILENCE_VALUE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="DEF_DIZZY_VALUE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="DEF_FREZE_VALUE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="MOVE_SPEED" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="ATK_SPEED" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="EQUIP_SCALE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="ESSENCE_SCALE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="GOLD_SCALE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="PHYSICAL_BREAK" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="VPREGEN" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="MAXHP_ADD_RATE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="ATK_ADD_RATE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="DEF_ADD_RATE" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="CRITICAL_ADD_RATE" form="unqualified" type="xsd:integer"/>
-              </xsd:complexType>
-            </xsd:element>
-          </xsd:sequence>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
-  <Map ID="1" Name="XML_映射" RootElement="XML" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
-  </Map>
-</MapInfo>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:AB4" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:AB4"/>
-  <tableColumns count="28">
-    <tableColumn id="1" uniqueName="ID" name="ID">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@ID" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="2" uniqueName="MAXHP" name="MAXHP">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@MAXHP" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="3" uniqueName="MAXSP" name="MAXSP">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@MAXSP" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="4" uniqueName="SpRegenTime" name="SpRegenTime">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@SpRegenTime" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="5" uniqueName="ATK_VALUE" name="ATK_VALUE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@ATK_VALUE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="6" uniqueName="DEF_VALUE" name="DEF_VALUE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@DEF_VALUE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="7" uniqueName="DODGE_VALUE" name="DODGE_VALUE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@DODGE_VALUE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="8" uniqueName="CRITICAL_VALUE" name="CRITICAL_VALUE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@CRITICAL_VALUE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="9" uniqueName="HPREGEN" name="HPREGEN">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@HPREGEN" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="10" uniqueName="CRITICAL_RATIO_VALUE" name="CRITICAL_RATIO_VALUE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@CRITICAL_RATIO_VALUE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="11" uniqueName="RESIST_VALUE" name="RESIST_VALUE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@RESIST_VALUE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="12" uniqueName="DEF_CRITICAL_RATIO_VALUE" name="DEF_CRITICAL_RATIO_VALUE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@DEF_CRITICAL_RATIO_VALUE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="13" uniqueName="DEF_HALT_VALUE" name="DEF_HALT_VALUE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@DEF_HALT_VALUE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="14" uniqueName="DEF_SLOW_VALUE" name="DEF_SLOW_VALUE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@DEF_SLOW_VALUE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="15" uniqueName="DEF_SILENCE_VALUE" name="DEF_SILENCE_VALUE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@DEF_SILENCE_VALUE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="16" uniqueName="DEF_DIZZY_VALUE" name="DEF_DIZZY_VALUE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@DEF_DIZZY_VALUE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="17" uniqueName="DEF_FREZE_VALUE" name="DEF_FREZE_VALUE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@DEF_FREZE_VALUE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="18" uniqueName="MOVE_SPEED" name="MOVE_SPEED">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@MOVE_SPEED" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="19" uniqueName="ATK_SPEED" name="ATK_SPEED">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@ATK_SPEED" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="20" uniqueName="EQUIP_SCALE" name="EQUIP_SCALE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@EQUIP_SCALE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="21" uniqueName="ESSENCE_SCALE" name="ESSENCE_SCALE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@ESSENCE_SCALE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="22" uniqueName="GOLD_SCALE" name="GOLD_SCALE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@GOLD_SCALE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="23" uniqueName="PHYSICAL_BREAK" name="PHYSICAL_BREAK">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@PHYSICAL_BREAK" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="24" uniqueName="VPREGEN" name="VPREGEN">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@VPREGEN" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="25" uniqueName="MAXHP_ADD_RATE" name="MAXHP_ADD_RATE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@MAXHP_ADD_RATE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="26" uniqueName="ATK_ADD_RATE" name="ATK_ADD_RATE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@ATK_ADD_RATE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="27" uniqueName="DEF_ADD_RATE" name="DEF_ADD_RATE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@DEF_ADD_RATE" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="28" uniqueName="CRITICAL_ADD_RATE" name="CRITICAL_ADD_RATE">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@CRITICAL_ADD_RATE" xmlDataType="integer"/>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -371,106 +201,106 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Cans" typeface="Euphemia"/>
         <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
         <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -482,181 +312,247 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:satMod val="350000"/>
+                <a:shade val="99000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="_h" fmla="val 21600"/>
+            <a:gd name="_w" fmla="val 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:pathLst>
+            <a:path w="21600" h="21600"/>
+          </a:pathLst>
+        </a:custGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:srgbClr val="9CBEE0"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="739CC3"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="200000"/>
+        </a:ln>
+      </a:spPr>
+      <a:bodyPr/>
+      <a:lstStyle/>
+    </a:spDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="2" max="3" width="9.375" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="20.25" customWidth="1"/>
+    <col min="9" max="9" width="11.625" customWidth="1"/>
+    <col min="10" max="10" width="27.75" customWidth="1"/>
+    <col min="11" max="11" width="17.75" customWidth="1"/>
+    <col min="12" max="12" width="32.75" customWidth="1"/>
+    <col min="13" max="14" width="20.25" customWidth="1"/>
+    <col min="15" max="15" width="24" customWidth="1"/>
+    <col min="16" max="17" width="21.5" customWidth="1"/>
+    <col min="18" max="18" width="15.25" customWidth="1"/>
+    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="20" max="20" width="16.5" customWidth="1"/>
+    <col min="21" max="21" width="19" customWidth="1"/>
+    <col min="22" max="22" width="15.25" customWidth="1"/>
+    <col min="23" max="23" width="20.25" customWidth="1"/>
+    <col min="24" max="24" width="11.625" customWidth="1"/>
+    <col min="25" max="25" width="20.25" customWidth="1"/>
+    <col min="26" max="27" width="17.75" customWidth="1"/>
+    <col min="28" max="28" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:28">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -742,7 +638,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -826,7 +722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -910,7 +806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -995,10 +891,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add language id for property name
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/EffectData.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/EffectData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherish\Desktop\git\nf\develop\_Out\Server\NFDataCfg\Excel_Ini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Desktop/NoahGameFrame/_Out/Server/NFDataCfg/Excel_Ini/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="13050"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27780" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,14 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -138,93 +146,6 @@
     <t>Desc</t>
   </si>
   <si>
-    <t>吸血</t>
-  </si>
-  <si>
-    <t>反伤</t>
-  </si>
-  <si>
-    <t>暴击</t>
-  </si>
-  <si>
-    <t>生命值</t>
-  </si>
-  <si>
-    <t>法力值</t>
-  </si>
-  <si>
-    <t>体力</t>
-  </si>
-  <si>
-    <t>生命值回复</t>
-  </si>
-  <si>
-    <t>体力回复</t>
-  </si>
-  <si>
-    <t>MP回复</t>
-  </si>
-  <si>
-    <t>物理攻击力</t>
-  </si>
-  <si>
-    <t>物理防御力</t>
-  </si>
-  <si>
-    <t>移动速度,默认单位是10000=1米</t>
-  </si>
-  <si>
-    <t>攻击速度默认10000</t>
-  </si>
-  <si>
-    <t>火</t>
-  </si>
-  <si>
-    <t>雷电</t>
-  </si>
-  <si>
-    <t>土</t>
-  </si>
-  <si>
-    <t>冰</t>
-  </si>
-  <si>
-    <t>毒</t>
-  </si>
-  <si>
-    <t>火抗</t>
-  </si>
-  <si>
-    <t>雷电抗</t>
-  </si>
-  <si>
-    <t>土抗</t>
-  </si>
-  <si>
-    <t>冰抗</t>
-  </si>
-  <si>
-    <t>毒抗</t>
-  </si>
-  <si>
-    <t>眩晕开关</t>
-  </si>
-  <si>
-    <t>移动开关</t>
-  </si>
-  <si>
-    <t>技能开关</t>
-  </si>
-  <si>
-    <t>物理免疫开关</t>
-  </si>
-  <si>
-    <t>魔法免疫开关</t>
-  </si>
-  <si>
-    <t>BUFF免疫开关</t>
-  </si>
-  <si>
     <t>PlayerAtt1</t>
   </si>
   <si>
@@ -455,12 +376,99 @@
   <si>
     <t>Upload</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LPID_SUCKBLOOD</t>
+  </si>
+  <si>
+    <t>LPID_REFLECTDAMAGE</t>
+  </si>
+  <si>
+    <t>LPID_CRITICAL</t>
+  </si>
+  <si>
+    <t>LPID_MAXHP</t>
+  </si>
+  <si>
+    <t>LPID_MAXMP</t>
+  </si>
+  <si>
+    <t>LPID_MAXSP</t>
+  </si>
+  <si>
+    <t>LPID_HPREGEN</t>
+  </si>
+  <si>
+    <t>LPID_SPREGEN</t>
+  </si>
+  <si>
+    <t>LPID_MPREGEN</t>
+  </si>
+  <si>
+    <t>LPID_ATK_VALUE</t>
+  </si>
+  <si>
+    <t>LPID_DEF_VALUE</t>
+  </si>
+  <si>
+    <t>LPID_MOVE_SPEED</t>
+  </si>
+  <si>
+    <t>LPID_ATK_SPEED</t>
+  </si>
+  <si>
+    <t>LPID_ATK_FIRE</t>
+  </si>
+  <si>
+    <t>LPID_ATK_LIGHT</t>
+  </si>
+  <si>
+    <t>LPID_ATK_WIND</t>
+  </si>
+  <si>
+    <t>LPID_ATK_ICE</t>
+  </si>
+  <si>
+    <t>LPID_ATK_POISON</t>
+  </si>
+  <si>
+    <t>LPID_DEF_FIRE</t>
+  </si>
+  <si>
+    <t>LPID_DEF_LIGHT</t>
+  </si>
+  <si>
+    <t>LPID_DEF_WIND</t>
+  </si>
+  <si>
+    <t>LPID_DEF_ICE</t>
+  </si>
+  <si>
+    <t>LPID_DEF_POISON</t>
+  </si>
+  <si>
+    <t>LPID_DIZZY_GATE</t>
+  </si>
+  <si>
+    <t>LPID_MOVE_GATE</t>
+  </si>
+  <si>
+    <t>LPID_SKILL_GATE</t>
+  </si>
+  <si>
+    <t>LPID_PHYSICAL_GATE</t>
+  </si>
+  <si>
+    <t>LPID_MAGIC_GATE</t>
+  </si>
+  <si>
+    <t>LPID_BUFF_GATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -676,7 +684,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -695,7 +703,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2">
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7">
     <tableStyle name="MySqlDefault" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
@@ -1044,24 +1052,28 @@
   <dimension ref="A1:AD85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="U10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="AD9" sqref="AD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" customWidth="1"/>
-    <col min="2" max="4" width="9.36328125" customWidth="1"/>
-    <col min="5" max="7" width="11.6328125" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="7" width="11.6640625" customWidth="1"/>
     <col min="8" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="15.26953125" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="26" width="16.453125" customWidth="1"/>
+    <col min="12" max="26" width="16.5" customWidth="1"/>
+    <col min="27" max="27" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1153,7 +1165,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>30</v>
       </c>
@@ -1245,7 +1257,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>32</v>
       </c>
@@ -1337,7 +1349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>33</v>
       </c>
@@ -1429,7 +1441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>34</v>
       </c>
@@ -1521,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>35</v>
       </c>
@@ -1613,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
@@ -1705,9 +1717,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -1797,101 +1809,101 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q9" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S9" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="T9" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="U9" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="V9" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="W9" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="X9" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y9" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z9" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA9" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB9" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC9" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD9" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A10" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="P9" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q9" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="R9" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="S9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="T9" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="U9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="V9" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="W9" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="X9" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y9" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA9" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB9" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC9" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD9" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1981,9 +1993,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2073,9 +2085,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2165,9 +2177,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2257,9 +2269,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2349,9 +2361,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2441,9 +2453,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -2533,9 +2545,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A17" s="12" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2625,9 +2637,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -2717,9 +2729,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A19" s="12" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -2809,9 +2821,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A20" s="12" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -2901,9 +2913,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -2993,9 +3005,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -3085,9 +3097,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -3177,9 +3189,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -3269,9 +3281,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -3361,9 +3373,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -3453,9 +3465,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -3545,9 +3557,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -3637,9 +3649,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -3729,9 +3741,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A30" s="12" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -3821,9 +3833,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A31" s="12" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -3913,9 +3925,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A32" s="12" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -4005,9 +4017,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A33" s="12" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -4097,9 +4109,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A34" s="12" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -4189,9 +4201,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -4281,9 +4293,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A36" s="12" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -4373,9 +4385,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A37" s="12" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -4465,9 +4477,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A38" s="12" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -4557,9 +4569,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A39" s="12" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -4649,9 +4661,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A40" s="12" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -4741,9 +4753,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A41" s="12" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -4833,9 +4845,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A42" s="12" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -4925,9 +4937,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A43" s="12" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -5017,9 +5029,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A44" s="12" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -5109,9 +5121,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A45" s="12" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -5201,9 +5213,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A46" s="12" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -5293,9 +5305,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A47" s="12" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -5385,9 +5397,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A48" s="12" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -5477,9 +5489,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A49" s="12" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -5569,9 +5581,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A50" s="12" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -5661,9 +5673,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A51" s="12" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -5753,9 +5765,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A52" s="12" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -5845,9 +5857,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A53" s="12" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -5937,9 +5949,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A54" s="12" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -6029,9 +6041,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A55" s="12" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -6121,9 +6133,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A56" s="12" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -6213,9 +6225,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A57" s="12" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -6305,9 +6317,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A58" s="12" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -6397,9 +6409,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A59" s="12" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -6489,9 +6501,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A60" s="12" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -6581,9 +6593,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A61" s="12" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -6673,9 +6685,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A62" s="12" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -6765,9 +6777,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A63" s="12" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -6857,9 +6869,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A64" s="12" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -6949,9 +6961,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A65" s="12" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -7041,9 +7053,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A66" s="12" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -7133,9 +7145,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A67" s="12" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -7225,9 +7237,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A68" s="12" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -7317,9 +7329,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A69" s="12" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -7409,9 +7421,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A70" s="12" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -7501,9 +7513,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A71" s="12" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -7593,9 +7605,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A72" s="12" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -7685,9 +7697,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A73" s="12" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -7777,9 +7789,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A74" s="12" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -7869,9 +7881,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A75" s="12" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -7961,9 +7973,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A76" s="12" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -8053,9 +8065,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A77" s="12" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -8145,9 +8157,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A78" s="12" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -8237,9 +8249,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A79" s="12" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -8329,9 +8341,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A80" s="12" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -8421,9 +8433,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A81" s="12" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -8513,9 +8525,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A82" s="12" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -8605,9 +8617,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A83" s="12" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -8697,9 +8709,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A84" s="12" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -8789,9 +8801,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A85" s="12" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="B85">
         <v>0</v>

</xml_diff>